<commit_message>
trying out html front landing
</commit_message>
<xml_diff>
--- a/excel_reports/_Summary_Info.xlsx
+++ b/excel_reports/_Summary_Info.xlsx
@@ -589,7 +589,7 @@
         <v>202</v>
       </c>
       <c r="C2" s="3">
-        <v>253</v>
+        <v>320</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="M2" s="3">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="R2" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S2" s="3">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>779</v>
       </c>
       <c r="C3" s="3">
-        <v>925</v>
+        <v>976</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="3">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="K3" s="4">
         <f>J3 * 2.5</f>
@@ -696,7 +696,7 @@
         <v>83</v>
       </c>
       <c r="M3" s="3">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>498</v>
       </c>
       <c r="C4" s="3">
-        <v>561</v>
+        <v>636</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K4" s="4">
         <f>J4 * 2.5</f>
@@ -769,7 +769,7 @@
         <v>104</v>
       </c>
       <c r="M4" s="3">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -786,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="R4" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S4" s="3">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>202</v>
       </c>
       <c r="C5" s="3">
-        <v>246</v>
+        <v>301</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -842,7 +842,7 @@
         <v>35</v>
       </c>
       <c r="M5" s="3">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>12</v>
       </c>
       <c r="R5" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S5" s="3">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
         <f>J6 * 2.5</f>
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>713</v>
       </c>
       <c r="C7" s="3">
-        <v>892</v>
+        <v>958</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="K7" s="4">
         <f>J7 * 2.5</f>
@@ -984,10 +984,10 @@
         <v>208</v>
       </c>
       <c r="M7" s="3">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="N7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="3">
         <f>-1*L7+M7+ N7</f>
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="R7" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>774</v>
       </c>
       <c r="C8" s="3">
-        <v>853</v>
+        <v>928</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="K8" s="4">
         <f>J8 * 2.5</f>
@@ -1057,7 +1057,7 @@
         <v>104</v>
       </c>
       <c r="M8" s="3">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="N8" s="3">
         <v>1</v>
@@ -1096,7 +1096,7 @@
         <v>271</v>
       </c>
       <c r="C9" s="3">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>62</v>
       </c>
       <c r="M9" s="3">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="N9" s="3">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>386</v>
       </c>
       <c r="C10" s="3">
-        <v>441</v>
+        <v>489</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="K10" s="4">
         <f>J10 * 2.5</f>
@@ -1203,7 +1203,7 @@
         <v>65</v>
       </c>
       <c r="M10" s="3">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="N10" s="3">
         <v>0</v>
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10" s="3">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>324</v>
       </c>
       <c r="C11" s="3">
-        <v>382</v>
+        <v>450</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
         <f>J11 * 2.5</f>
@@ -1276,7 +1276,7 @@
         <v>74</v>
       </c>
       <c r="M11" s="3">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="N11" s="3">
         <v>0</v>
@@ -1293,7 +1293,7 @@
         <v>18</v>
       </c>
       <c r="R11" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S11" s="3">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         <v>248</v>
       </c>
       <c r="C12" s="3">
-        <v>303</v>
+        <v>398</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>45</v>
       </c>
       <c r="M12" s="3">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="N12" s="3">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="R12" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S12" s="3">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="3">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="3">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="N13" s="3">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="3">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="3">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1495,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="M14" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N14" s="3">
         <v>0</v>
@@ -1530,7 +1530,7 @@
         <v>605</v>
       </c>
       <c r="C15" s="3">
-        <v>657</v>
+        <v>734</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="K15" s="4">
         <f>J15 * 2.5</f>
@@ -1564,7 +1564,7 @@
         <v>104</v>
       </c>
       <c r="M15" s="3">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="N15" s="3">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>648</v>
       </c>
       <c r="C16" s="3">
-        <v>832</v>
+        <v>881</v>
       </c>
       <c r="D16" s="3">
         <v>5</v>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="K16" s="4">
         <f>J16 * 2.5</f>
@@ -1637,7 +1637,7 @@
         <v>88</v>
       </c>
       <c r="M16" s="3">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="N16" s="3">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>17</v>
       </c>
       <c r="R16" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <v>490</v>
       </c>
       <c r="C17" s="3">
-        <v>534</v>
+        <v>586</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="K17" s="4">
         <f>J17 * 2.5</f>
@@ -1710,7 +1710,7 @@
         <v>106</v>
       </c>
       <c r="M17" s="3">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="N17" s="3">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         <v>604</v>
       </c>
       <c r="C18" s="3">
-        <v>661</v>
+        <v>748</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
@@ -1769,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="K18" s="4">
         <f>J18 * 2.5</f>
@@ -1779,7 +1779,7 @@
         <v>96</v>
       </c>
       <c r="M18" s="3">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="N18" s="3">
         <v>1</v>
@@ -1818,7 +1818,7 @@
         <v>505</v>
       </c>
       <c r="C19" s="3">
-        <v>576</v>
+        <v>622</v>
       </c>
       <c r="D19" s="3">
         <v>0</v>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="K19" s="4">
         <f>J19 * 2.5</f>
@@ -1852,7 +1852,7 @@
         <v>85</v>
       </c>
       <c r="M19" s="3">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N19" s="3">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>410</v>
       </c>
       <c r="C20" s="3">
-        <v>457</v>
+        <v>505</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="K20" s="4">
         <f>J20 * 2.5</f>
@@ -1925,7 +1925,7 @@
         <v>67</v>
       </c>
       <c r="M20" s="3">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="N20" s="3">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>876</v>
       </c>
       <c r="C21" s="3">
-        <v>1097</v>
+        <v>1143</v>
       </c>
       <c r="D21" s="3">
         <v>3</v>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>483</v>
+        <v>518</v>
       </c>
       <c r="K21" s="4">
         <f>J21 * 2.5</f>
@@ -1998,7 +1998,7 @@
         <v>92</v>
       </c>
       <c r="M21" s="3">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N21" s="3">
         <v>0</v>
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S21" s="3">
         <v>0</v>
@@ -2037,7 +2037,7 @@
         <v>542</v>
       </c>
       <c r="C22" s="3">
-        <v>625</v>
+        <v>635</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="K22" s="4">
         <f>J22 * 2.5</f>
@@ -2071,7 +2071,7 @@
         <v>50</v>
       </c>
       <c r="M22" s="3">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="N22" s="3">
         <v>0</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="K23" s="4">
         <f>J23 * 2.5</f>
@@ -2183,7 +2183,7 @@
         <v>244</v>
       </c>
       <c r="C24" s="3">
-        <v>319</v>
+        <v>388</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -2217,7 +2217,7 @@
         <v>60</v>
       </c>
       <c r="M24" s="3">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>14</v>
       </c>
       <c r="R24" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S24" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
tweak adding in cancels
</commit_message>
<xml_diff>
--- a/excel_reports/_Summary_Info.xlsx
+++ b/excel_reports/_Summary_Info.xlsx
@@ -586,10 +586,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="3">
-        <v>202</v>
+        <v>327</v>
       </c>
       <c r="C2" s="3">
-        <v>327</v>
+        <v>252</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="3">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="M2" s="3">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
@@ -637,10 +637,10 @@
         <v>0</v>
       </c>
       <c r="Q2" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R2" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S2" s="3">
         <v>0</v>
@@ -659,13 +659,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="3">
-        <v>779</v>
+        <v>973</v>
       </c>
       <c r="C3" s="3">
-        <v>975</v>
+        <v>914</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <f>-1*B3+C3+D3</f>
@@ -686,17 +686,17 @@
         <v>0</v>
       </c>
       <c r="J3" s="3">
-        <v>377</v>
+        <v>344</v>
       </c>
       <c r="K3" s="4">
         <f>J3 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L3" s="3">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="M3" s="3">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="N3" s="3">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R3" s="3">
         <v>27</v>
@@ -732,10 +732,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="3">
-        <v>498</v>
+        <v>637</v>
       </c>
       <c r="C4" s="3">
-        <v>637</v>
+        <v>561</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -759,17 +759,17 @@
         <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K4" s="4">
         <f>J4 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="M4" s="3">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -783,10 +783,10 @@
         <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R4" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S4" s="3">
         <v>0</v>
@@ -805,10 +805,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="3">
-        <v>202</v>
+        <v>310</v>
       </c>
       <c r="C5" s="3">
-        <v>310</v>
+        <v>246</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -839,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="3">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="M5" s="3">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
@@ -856,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="Q5" s="3">
+        <v>16</v>
+      </c>
+      <c r="R5" s="3">
         <v>12</v>
-      </c>
-      <c r="R5" s="3">
-        <v>16</v>
       </c>
       <c r="S5" s="3">
         <v>0</v>
@@ -878,10 +878,10 @@
         <v>25</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="C6" s="3">
-        <v>150</v>
+        <v>66</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -912,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="3">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="M6" s="3">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
@@ -947,13 +947,13 @@
         <v>26</v>
       </c>
       <c r="B7" s="3">
-        <v>713</v>
+        <v>951</v>
       </c>
       <c r="C7" s="3">
-        <v>951</v>
+        <v>885</v>
       </c>
       <c r="D7" s="3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3">
         <f>-1*B7+C7+D7</f>
@@ -974,17 +974,17 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="K7" s="4">
         <f>J7 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L7" s="3">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="M7" s="3">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="N7" s="3">
         <v>3</v>
@@ -998,10 +998,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="R7" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -1020,13 +1020,13 @@
         <v>27</v>
       </c>
       <c r="B8" s="3">
-        <v>774</v>
+        <v>934</v>
       </c>
       <c r="C8" s="3">
-        <v>933</v>
+        <v>851</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <f>-1*B8+C8+D8</f>
@@ -1047,17 +1047,17 @@
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K8" s="4">
         <f>J8 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L8" s="3">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="M8" s="3">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="N8" s="3">
         <v>1</v>
@@ -1093,10 +1093,10 @@
         <v>28</v>
       </c>
       <c r="B9" s="3">
-        <v>271</v>
+        <v>388</v>
       </c>
       <c r="C9" s="3">
-        <v>388</v>
+        <v>316</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1127,10 +1127,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="M9" s="3">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N9" s="3">
         <v>0</v>
@@ -1166,10 +1166,10 @@
         <v>29</v>
       </c>
       <c r="B10" s="3">
-        <v>386</v>
+        <v>493</v>
       </c>
       <c r="C10" s="3">
-        <v>492</v>
+        <v>437</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1193,17 +1193,17 @@
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="K10" s="4">
         <f>J10 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L10" s="3">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="M10" s="3">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N10" s="3">
         <v>0</v>
@@ -1217,10 +1217,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="3">
+        <v>2</v>
+      </c>
+      <c r="R10" s="3">
         <v>1</v>
-      </c>
-      <c r="R10" s="3">
-        <v>2</v>
       </c>
       <c r="S10" s="3">
         <v>0</v>
@@ -1239,10 +1239,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="3">
-        <v>324</v>
+        <v>453</v>
       </c>
       <c r="C11" s="3">
-        <v>452</v>
+        <v>377</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1266,17 +1266,17 @@
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="4">
         <f>J11 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="M11" s="3">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="N11" s="3">
         <v>0</v>
@@ -1290,10 +1290,10 @@
         <v>0</v>
       </c>
       <c r="Q11" s="3">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="R11" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S11" s="3">
         <v>0</v>
@@ -1312,10 +1312,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="3">
-        <v>248</v>
+        <v>397</v>
       </c>
       <c r="C12" s="3">
-        <v>397</v>
+        <v>299</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1346,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="3">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="M12" s="3">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="N12" s="3">
         <v>0</v>
@@ -1363,10 +1363,10 @@
         <v>0</v>
       </c>
       <c r="Q12" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R12" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S12" s="3">
         <v>0</v>
@@ -1385,10 +1385,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="3">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="C13" s="3">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1412,17 +1412,17 @@
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="4">
         <f>J13 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L13" s="3">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M13" s="3">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="N13" s="3">
         <v>0</v>
@@ -1436,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="Q13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="3">
         <v>0</v>
@@ -1458,10 +1458,10 @@
         <v>33</v>
       </c>
       <c r="B14" s="3">
-        <v>36</v>
+        <v>154</v>
       </c>
       <c r="C14" s="3">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1492,10 +1492,10 @@
         <v>0</v>
       </c>
       <c r="L14" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="M14" s="3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="N14" s="3">
         <v>0</v>
@@ -1527,13 +1527,13 @@
         <v>34</v>
       </c>
       <c r="B15" s="3">
-        <v>605</v>
+        <v>736</v>
       </c>
       <c r="C15" s="3">
-        <v>736</v>
+        <v>652</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
         <f>-1*B15+C15+D15</f>
@@ -1554,17 +1554,17 @@
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="K15" s="4">
         <f>J15 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L15" s="3">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="M15" s="3">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="N15" s="3">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R15" s="3">
         <v>30</v>
@@ -1600,13 +1600,13 @@
         <v>35</v>
       </c>
       <c r="B16" s="3">
-        <v>648</v>
+        <v>883</v>
       </c>
       <c r="C16" s="3">
-        <v>885</v>
+        <v>832</v>
       </c>
       <c r="D16" s="3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3">
         <f>-1*B16+C16+D16</f>
@@ -1627,17 +1627,17 @@
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="K16" s="4">
         <f>J16 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="M16" s="3">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="N16" s="3">
         <v>0</v>
@@ -1651,10 +1651,10 @@
         <v>0</v>
       </c>
       <c r="Q16" s="3">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="R16" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -1673,10 +1673,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="3">
-        <v>490</v>
+        <v>591</v>
       </c>
       <c r="C17" s="3">
-        <v>591</v>
+        <v>533</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -1700,17 +1700,17 @@
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="K17" s="4">
         <f>J17 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L17" s="3">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="M17" s="3">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="N17" s="3">
         <v>0</v>
@@ -1742,10 +1742,10 @@
         <v>37</v>
       </c>
       <c r="B18" s="3">
-        <v>604</v>
+        <v>745</v>
       </c>
       <c r="C18" s="3">
-        <v>746</v>
+        <v>656</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -1769,17 +1769,17 @@
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="K18" s="4">
         <f>J18 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L18" s="3">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="M18" s="3">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="N18" s="3">
         <v>5</v>
@@ -1815,13 +1815,13 @@
         <v>38</v>
       </c>
       <c r="B19" s="3">
-        <v>505</v>
+        <v>623</v>
       </c>
       <c r="C19" s="3">
-        <v>626</v>
+        <v>574</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3">
         <f>-1*B19+C19+D19</f>
@@ -1842,17 +1842,17 @@
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="K19" s="4">
         <f>J19 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L19" s="3">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="M19" s="3">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="N19" s="3">
         <v>0</v>
@@ -1888,13 +1888,13 @@
         <v>39</v>
       </c>
       <c r="B20" s="3">
-        <v>410</v>
+        <v>508</v>
       </c>
       <c r="C20" s="3">
-        <v>508</v>
+        <v>455</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
         <f>-1*B20+C20+D20</f>
@@ -1915,17 +1915,17 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="K20" s="4">
         <f>J20 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L20" s="3">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="M20" s="3">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="N20" s="3">
         <v>0</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R20" s="3">
         <v>8</v>
@@ -1961,13 +1961,13 @@
         <v>40</v>
       </c>
       <c r="B21" s="3">
-        <v>876</v>
+        <v>1142</v>
       </c>
       <c r="C21" s="3">
-        <v>1142</v>
+        <v>1089</v>
       </c>
       <c r="D21" s="3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E21" s="3">
         <f>-1*B21+C21+D21</f>
@@ -1988,17 +1988,17 @@
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>516</v>
+        <v>480</v>
       </c>
       <c r="K21" s="4">
         <f>J21 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L21" s="3">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="M21" s="3">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="N21" s="3">
         <v>0</v>
@@ -2012,10 +2012,10 @@
         <v>0</v>
       </c>
       <c r="Q21" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R21" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S21" s="3">
         <v>0</v>
@@ -2034,13 +2034,13 @@
         <v>41</v>
       </c>
       <c r="B22" s="3">
-        <v>542</v>
+        <v>630</v>
       </c>
       <c r="C22" s="3">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="D22" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E22" s="3">
         <f>-1*B22+C22+D22</f>
@@ -2061,17 +2061,17 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>319</v>
+        <v>287</v>
       </c>
       <c r="K22" s="4">
         <f>J22 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L22" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M22" s="3">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="N22" s="3">
         <v>0</v>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="3">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="R22" s="3">
         <v>15</v>
@@ -2107,13 +2107,13 @@
         <v>42</v>
       </c>
       <c r="B23" s="3">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="C23" s="3">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="3">
         <f>-1*B23+C23+D23</f>
@@ -2134,17 +2134,17 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="K23" s="4">
         <f>J23 * 2.5</f>
         <v>0</v>
       </c>
       <c r="L23" s="3">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="M23" s="3">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N23" s="3">
         <v>1</v>
@@ -2180,10 +2180,10 @@
         <v>43</v>
       </c>
       <c r="B24" s="3">
-        <v>244</v>
+        <v>388</v>
       </c>
       <c r="C24" s="3">
-        <v>388</v>
+        <v>315</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -2214,10 +2214,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="3">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="M24" s="3">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
@@ -2231,10 +2231,10 @@
         <v>0</v>
       </c>
       <c r="Q24" s="3">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="R24" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S24" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
fix originating agent for ancillaries
</commit_message>
<xml_diff>
--- a/excel_reports/_Summary_Info.xlsx
+++ b/excel_reports/_Summary_Info.xlsx
@@ -589,7 +589,7 @@
         <v>327</v>
       </c>
       <c r="C2" s="3">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="3">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
@@ -640,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="R2" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S2" s="3">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>973</v>
       </c>
       <c r="C3" s="3">
-        <v>914</v>
+        <v>976</v>
       </c>
       <c r="D3" s="3">
         <v>11</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="3">
-        <v>344</v>
+        <v>377</v>
       </c>
       <c r="K3" s="4">
         <f>J3 * 2.5</f>
@@ -696,7 +696,7 @@
         <v>108</v>
       </c>
       <c r="M3" s="3">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="N3" s="3">
         <v>1</v>
@@ -735,7 +735,7 @@
         <v>637</v>
       </c>
       <c r="C4" s="3">
-        <v>561</v>
+        <v>637</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K4" s="4">
         <f>J4 * 2.5</f>
@@ -769,7 +769,7 @@
         <v>124</v>
       </c>
       <c r="M4" s="3">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -786,7 +786,7 @@
         <v>11</v>
       </c>
       <c r="R4" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S4" s="3">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>310</v>
       </c>
       <c r="C5" s="3">
-        <v>246</v>
+        <v>310</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -842,7 +842,7 @@
         <v>53</v>
       </c>
       <c r="M5" s="3">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="R5" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S5" s="3">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>150</v>
       </c>
       <c r="C6" s="3">
-        <v>66</v>
+        <v>152</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
         <f>J6 * 2.5</f>
@@ -915,7 +915,7 @@
         <v>28</v>
       </c>
       <c r="M6" s="3">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
@@ -950,7 +950,7 @@
         <v>951</v>
       </c>
       <c r="C7" s="3">
-        <v>885</v>
+        <v>952</v>
       </c>
       <c r="D7" s="3">
         <v>14</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>355</v>
+        <v>374</v>
       </c>
       <c r="K7" s="4">
         <f>J7 * 2.5</f>
@@ -984,7 +984,7 @@
         <v>237</v>
       </c>
       <c r="M7" s="3">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="N7" s="3">
         <v>3</v>
@@ -1001,7 +1001,7 @@
         <v>17</v>
       </c>
       <c r="R7" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S7" s="3">
         <v>0</v>
@@ -1023,10 +1023,10 @@
         <v>934</v>
       </c>
       <c r="C8" s="3">
-        <v>851</v>
+        <v>933</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
         <f>-1*B8+C8+D8</f>
@@ -1047,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="3">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="K8" s="4">
         <f>J8 * 2.5</f>
@@ -1057,7 +1057,7 @@
         <v>125</v>
       </c>
       <c r="M8" s="3">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="N8" s="3">
         <v>1</v>
@@ -1096,7 +1096,7 @@
         <v>388</v>
       </c>
       <c r="C9" s="3">
-        <v>316</v>
+        <v>389</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>86</v>
       </c>
       <c r="M9" s="3">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="N9" s="3">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>493</v>
       </c>
       <c r="C10" s="3">
-        <v>437</v>
+        <v>493</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="K10" s="4">
         <f>J10 * 2.5</f>
@@ -1203,7 +1203,7 @@
         <v>79</v>
       </c>
       <c r="M10" s="3">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="N10" s="3">
         <v>0</v>
@@ -1220,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="R10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10" s="3">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>453</v>
       </c>
       <c r="C11" s="3">
-        <v>377</v>
+        <v>454</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
         <f>J11 * 2.5</f>
@@ -1276,7 +1276,7 @@
         <v>105</v>
       </c>
       <c r="M11" s="3">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="N11" s="3">
         <v>0</v>
@@ -1293,7 +1293,7 @@
         <v>22</v>
       </c>
       <c r="R11" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S11" s="3">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         <v>397</v>
       </c>
       <c r="C12" s="3">
-        <v>299</v>
+        <v>397</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>69</v>
       </c>
       <c r="M12" s="3">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="N12" s="3">
         <v>0</v>
@@ -1366,7 +1366,7 @@
         <v>5</v>
       </c>
       <c r="R12" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S12" s="3">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>110</v>
       </c>
       <c r="C13" s="3">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1412,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="4">
         <f>J13 * 2.5</f>
@@ -1422,7 +1422,7 @@
         <v>23</v>
       </c>
       <c r="M13" s="3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="N13" s="3">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="R13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="3">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>154</v>
       </c>
       <c r="C14" s="3">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1495,7 +1495,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N14" s="3">
         <v>0</v>
@@ -1530,7 +1530,7 @@
         <v>736</v>
       </c>
       <c r="C15" s="3">
-        <v>652</v>
+        <v>737</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="K15" s="4">
         <f>J15 * 2.5</f>
@@ -1564,7 +1564,7 @@
         <v>133</v>
       </c>
       <c r="M15" s="3">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="N15" s="3">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>883</v>
       </c>
       <c r="C16" s="3">
-        <v>832</v>
+        <v>883</v>
       </c>
       <c r="D16" s="3">
         <v>21</v>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <v>372</v>
+        <v>393</v>
       </c>
       <c r="K16" s="4">
         <f>J16 * 2.5</f>
@@ -1637,7 +1637,7 @@
         <v>110</v>
       </c>
       <c r="M16" s="3">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="N16" s="3">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="R16" s="3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="S16" s="3">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <v>591</v>
       </c>
       <c r="C17" s="3">
-        <v>533</v>
+        <v>591</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="K17" s="4">
         <f>J17 * 2.5</f>
@@ -1710,7 +1710,7 @@
         <v>116</v>
       </c>
       <c r="M17" s="3">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N17" s="3">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         <v>745</v>
       </c>
       <c r="C18" s="3">
-        <v>656</v>
+        <v>746</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -1769,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="K18" s="4">
         <f>J18 * 2.5</f>
@@ -1779,7 +1779,7 @@
         <v>133</v>
       </c>
       <c r="M18" s="3">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="N18" s="3">
         <v>5</v>
@@ -1818,7 +1818,7 @@
         <v>623</v>
       </c>
       <c r="C19" s="3">
-        <v>574</v>
+        <v>626</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="K19" s="4">
         <f>J19 * 2.5</f>
@@ -1852,7 +1852,7 @@
         <v>103</v>
       </c>
       <c r="M19" s="3">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="N19" s="3">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>508</v>
       </c>
       <c r="C20" s="3">
-        <v>455</v>
+        <v>508</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="K20" s="4">
         <f>J20 * 2.5</f>
@@ -1925,7 +1925,7 @@
         <v>77</v>
       </c>
       <c r="M20" s="3">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N20" s="3">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>1142</v>
       </c>
       <c r="C21" s="3">
-        <v>1089</v>
+        <v>1144</v>
       </c>
       <c r="D21" s="3">
         <v>16</v>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <v>480</v>
+        <v>518</v>
       </c>
       <c r="K21" s="4">
         <f>J21 * 2.5</f>
@@ -1998,7 +1998,7 @@
         <v>101</v>
       </c>
       <c r="M21" s="3">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N21" s="3">
         <v>0</v>
@@ -2015,7 +2015,7 @@
         <v>3</v>
       </c>
       <c r="R21" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S21" s="3">
         <v>0</v>
@@ -2037,7 +2037,7 @@
         <v>630</v>
       </c>
       <c r="C22" s="3">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="D22" s="3">
         <v>9</v>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>287</v>
+        <v>319</v>
       </c>
       <c r="K22" s="4">
         <f>J22 * 2.5</f>
@@ -2071,7 +2071,7 @@
         <v>60</v>
       </c>
       <c r="M22" s="3">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="N22" s="3">
         <v>0</v>
@@ -2110,7 +2110,7 @@
         <v>429</v>
       </c>
       <c r="C23" s="3">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="K23" s="4">
         <f>J23 * 2.5</f>
@@ -2144,7 +2144,7 @@
         <v>114</v>
       </c>
       <c r="M23" s="3">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="N23" s="3">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>388</v>
       </c>
       <c r="C24" s="3">
-        <v>315</v>
+        <v>388</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -2217,7 +2217,7 @@
         <v>83</v>
       </c>
       <c r="M24" s="3">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="N24" s="3">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="R24" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S24" s="3">
         <v>0</v>

</xml_diff>